<commit_message>
feat: mejoras en dashboard, flujo de credenciales, y UI/UX; fixes en creación de club, feedback modal, y estadísticas en admin
</commit_message>
<xml_diff>
--- a/Categorias.xlsx
+++ b/Categorias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\time4swim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E88CB5-516D-4A92-849D-B2BDEC11377A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F522984-914F-4D93-B0F9-3D404F87E3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03A3668F-D4D1-48D5-9CEA-3D109436E11D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Categoría</t>
   </si>
@@ -53,39 +53,18 @@
     <t>Pre-Mínima</t>
   </si>
   <si>
-    <t>pre_minima</t>
-  </si>
-  <si>
-    <t>2019 y posteriores</t>
-  </si>
-  <si>
-    <t>≤ 6 años</t>
-  </si>
-  <si>
     <t>Mínima 1</t>
   </si>
   <si>
     <t>minima_1</t>
   </si>
   <si>
-    <t>2017-2018</t>
-  </si>
-  <si>
-    <t>7-8 años</t>
-  </si>
-  <si>
     <t>Mínima 2</t>
   </si>
   <si>
     <t>minima_2</t>
   </si>
   <si>
-    <t>2015-2016</t>
-  </si>
-  <si>
-    <t>9-10 años</t>
-  </si>
-  <si>
     <t>Infantil A1</t>
   </si>
   <si>
@@ -146,33 +125,18 @@
     <t>juvenil_c</t>
   </si>
   <si>
-    <t>17 años</t>
-  </si>
-  <si>
     <t>Junior</t>
   </si>
   <si>
     <t>junior</t>
   </si>
   <si>
-    <t>2006-2007</t>
-  </si>
-  <si>
-    <t>18-19 años</t>
-  </si>
-  <si>
     <t>Senior</t>
   </si>
   <si>
     <t>senior</t>
   </si>
   <si>
-    <t>2001-2005</t>
-  </si>
-  <si>
-    <t>20-24 años</t>
-  </si>
-  <si>
     <t>Master</t>
   </si>
   <si>
@@ -183,13 +147,58 @@
   </si>
   <si>
     <t>25+ años</t>
+  </si>
+  <si>
+    <t>Baby Splash</t>
+  </si>
+  <si>
+    <t>2020 -2021</t>
+  </si>
+  <si>
+    <t>pre_minima_2</t>
+  </si>
+  <si>
+    <t>pre_minima_1</t>
+  </si>
+  <si>
+    <t>6 años</t>
+  </si>
+  <si>
+    <t>baby_splash</t>
+  </si>
+  <si>
+    <t>7 años</t>
+  </si>
+  <si>
+    <t>8 años</t>
+  </si>
+  <si>
+    <t>9 años</t>
+  </si>
+  <si>
+    <t>10 años</t>
+  </si>
+  <si>
+    <t>2008-2007</t>
+  </si>
+  <si>
+    <t>2006-2001</t>
+  </si>
+  <si>
+    <t>17-18 años</t>
+  </si>
+  <si>
+    <t>19-24 años</t>
+  </si>
+  <si>
+    <t>&lt; 5 años</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,22 +208,35 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD0D0D0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FFCCCCCC"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Segoe UI"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFD0D0D0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -258,19 +280,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,20 +635,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B58594-67A6-48F9-81D3-D27511A3BFAF}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" s="2" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,189 +664,221 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:5" s="2" customFormat="1" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2018</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D6" s="7">
+        <v>2017</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D7" s="7">
+        <v>2016</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D8" s="7">
+        <v>2015</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2014</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
+    <row r="10" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2013</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="11" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2012</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4">
-        <v>2014</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
+    </row>
+    <row r="12" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2011</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4">
-        <v>2013</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="13" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2010</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4">
-        <v>2012</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="14" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2009</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4">
-        <v>2011</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="3" t="s">
+    </row>
+    <row r="15" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4">
-        <v>2010</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+      <c r="D15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4">
-        <v>2009</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="4">
-        <v>2008</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="18" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>